<commit_message>
approximate computing exp sim
</commit_message>
<xml_diff>
--- a/unit/exp/software/sim_coeff_select_final_version/sim_coeff_selet_gradient_final_version_summary_gaussian_0.75_0.1.xlsx
+++ b/unit/exp/software/sim_coeff_select_final_version/sim_coeff_selet_gradient_final_version_summary_gaussian_0.75_0.1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wudidaizi/Project/approximate_computing/unit/exp/software/sim_coeff_select_final_version/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A055E92-BA83-1E4B-915A-96B28EB51096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4D0D86-7D0D-B94D-BBED-A78853606373}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sim_coeff_selet_gradient_final_" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -946,11 +946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,6 +1311,264 @@
         <v>28</v>
       </c>
     </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0.125</v>
+      </c>
+      <c r="D10">
+        <v>0.375</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <v>0.125</v>
+      </c>
+      <c r="I10">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>4</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>100000000000000</v>
+      </c>
+      <c r="V10">
+        <v>5.4495000000000002E-2</v>
+      </c>
+      <c r="W10">
+        <v>7.7980000000000002E-3</v>
+      </c>
+      <c r="X10">
+        <v>8.5389999999999997E-3</v>
+      </c>
+      <c r="Y10">
+        <v>8.5679999999999992E-3</v>
+      </c>
+      <c r="Z10">
+        <v>8.5679999999999992E-3</v>
+      </c>
+      <c r="AA10">
+        <v>8.5679999999999992E-3</v>
+      </c>
+      <c r="AB10">
+        <v>8.5679999999999992E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>0.125</v>
+      </c>
+      <c r="D11">
+        <v>0.375</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.5</v>
+      </c>
+      <c r="H11">
+        <v>0.125</v>
+      </c>
+      <c r="I11">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>100000000000000</v>
+      </c>
+      <c r="V11">
+        <v>4.5599000000000001E-2</v>
+      </c>
+      <c r="W11">
+        <v>4.5269999999999998E-3</v>
+      </c>
+      <c r="X11">
+        <v>6.9700000000000003E-4</v>
+      </c>
+      <c r="Y11">
+        <v>2.72E-4</v>
+      </c>
+      <c r="Z11">
+        <v>2.72E-4</v>
+      </c>
+      <c r="AA11">
+        <v>2.72E-4</v>
+      </c>
+      <c r="AB11">
+        <v>2.72E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0.125</v>
+      </c>
+      <c r="D12">
+        <v>0.375</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0.125</v>
+      </c>
+      <c r="I12">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>4</v>
+      </c>
+      <c r="T12">
+        <v>4</v>
+      </c>
+      <c r="U12">
+        <v>100000000000000</v>
+      </c>
+      <c r="V12">
+        <v>4.5058000000000001E-2</v>
+      </c>
+      <c r="W12">
+        <v>4.9750000000000003E-3</v>
+      </c>
+      <c r="X12">
+        <v>8.9899999999999995E-4</v>
+      </c>
+      <c r="Y12">
+        <v>2.7399999999999999E-4</v>
+      </c>
+      <c r="Z12">
+        <v>2.7399999999999999E-4</v>
+      </c>
+      <c r="AA12">
+        <v>2.7399999999999999E-4</v>
+      </c>
+      <c r="AB12">
+        <v>2.7399999999999999E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>